<commit_message>
migrated necessary data / fixed ext1 report
</commit_message>
<xml_diff>
--- a/tbs/templates/IMT_EXT1.xlsx
+++ b/tbs/templates/IMT_EXT1.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\imt\production\tbs\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\imt\tbs\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30546883-3962-4850-A2D1-A62C8739237B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="R_A1" sheetId="1" r:id="rId1"/>
@@ -19,12 +18,12 @@
   <definedNames>
     <definedName name="the_named_cell">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>This sheet was hidden in the template, and it becomes visible.</t>
   </si>
@@ -98,12 +97,6 @@
     <t>[a.HOUSEHOLD_ID;block=tbs:row]</t>
   </si>
   <si>
-    <t>[a.col1;ope=tbs:num]</t>
-  </si>
-  <si>
-    <t>[a.col2;ope=tbs:num]</t>
-  </si>
-  <si>
     <t>[a.YDS;ope=tbs:num]</t>
   </si>
   <si>
@@ -113,12 +106,6 @@
     <t>Area : [onshow.a_coverage]</t>
   </si>
   <si>
-    <t>DTI/Government Financial Institutions (Microcredit/ microfinance)</t>
-  </si>
-  <si>
-    <t>DA  (Assistance to Pantawid farmer benefeciaries</t>
-  </si>
-  <si>
     <t>External Interventions (Other Government Agencies)</t>
   </si>
   <si>
@@ -128,16 +115,136 @@
     <t>[a.LOWB]</t>
   </si>
   <si>
-    <t>Other Interventions</t>
-  </si>
-  <si>
-    <t>[a.col3;ope=tbs:num]</t>
+    <t>Department of Agriculture (DA)</t>
+  </si>
+  <si>
+    <t>[a.da1;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>[a.da2;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>[a.da3;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>[a.da4;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>[a.da5;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>[a.da6;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>Assistance to Pantawid farmer benefeciaries</t>
+  </si>
+  <si>
+    <t>Enhanced National Greening Program</t>
+  </si>
+  <si>
+    <t>Rice Resiliency Project</t>
+  </si>
+  <si>
+    <t>Plant, Plant, Plant Program</t>
+  </si>
+  <si>
+    <t>Ahon Lahat, Pagkaing Sapat (ALPAS)</t>
+  </si>
+  <si>
+    <t>Agri-Negosyo (ANYO)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tulong Panghanapbuhay sa Ating Disadvantaged/Displaced Workers (TUPAD) </t>
+  </si>
+  <si>
+    <t>Government Internship Program (GIP)</t>
+  </si>
+  <si>
+    <t>Emergency Employment Program (EEP)</t>
+  </si>
+  <si>
+    <t>DOLE Integrated Livelihood and Emergency Employment Program (DILEEP)</t>
+  </si>
+  <si>
+    <t>[a.dole1;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>[a.dole2;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>[a.dole3;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>[a.dole4;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>Department of Labor and Employment (DOLE)</t>
+  </si>
+  <si>
+    <t>Department of Trade and Industry (DTI)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Negosyo Centers </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shared Service Facilities (SSF) Program </t>
+  </si>
+  <si>
+    <t>Pondo sa Pagbabago at Pag-asenso (P3)</t>
+  </si>
+  <si>
+    <t>Kapatid Mentor Me Program (KMME)</t>
+  </si>
+  <si>
+    <t>One Town, One Product Philippines (OTOP)</t>
+  </si>
+  <si>
+    <t>[a.dti1;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>[a.dti2;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>[a.dti3;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>[a.dti4;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>[a.dti5;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>National Economic and Development Authority (NEDA)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AmBisyon Natin 2040 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Philippine Development Plan (PDP) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recharge PH: Philippine National Recharge Strategy for Sustainable Development </t>
+  </si>
+  <si>
+    <t>others</t>
+  </si>
+  <si>
+    <t>[a.neda1;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>[a.neda2;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>[a.neda3;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>[a.other;ope=tbs:num]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
@@ -270,7 +377,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -312,28 +419,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -347,47 +432,27 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right/>
+      <top style="thin">
         <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right style="thin">
         <color indexed="64"/>
-      </left>
-      <right/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
+      <bottom style="thin">
         <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -418,9 +483,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -434,24 +496,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -476,34 +559,16 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -605,23 +670,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -657,23 +705,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -849,92 +880,104 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AD14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.109375" customWidth="1"/>
-    <col min="2" max="5" width="18.44140625" customWidth="1"/>
-    <col min="6" max="8" width="16.5546875" customWidth="1"/>
-    <col min="12" max="13" width="22.88671875" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" customWidth="1"/>
+    <col min="2" max="5" width="18.42578125" customWidth="1"/>
+    <col min="6" max="8" width="16.5703125" customWidth="1"/>
+    <col min="12" max="17" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:30" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
     </row>
-    <row r="2" spans="1:14" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="26" t="s">
+    <row r="2" spans="1:30" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
     </row>
-    <row r="3" spans="1:14" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="28" t="s">
+    <row r="3" spans="1:30" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="20"/>
     </row>
-    <row r="4" spans="1:14" s="5" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="30" t="s">
+    <row r="4" spans="1:30" s="5" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
-      <c r="K4" s="31"/>
-      <c r="L4" s="31"/>
-      <c r="M4" s="31"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
+      <c r="M4" s="37"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="21"/>
+      <c r="P4" s="21"/>
     </row>
-    <row r="5" spans="1:14" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:30" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="8"/>
@@ -947,102 +990,196 @@
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
-      <c r="N5" s="9"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="9"/>
     </row>
-    <row r="6" spans="1:14" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:30" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="B6" s="6"/>
       <c r="C6" s="8"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
       <c r="I6" s="4"/>
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
-      <c r="N6" s="9"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="9"/>
     </row>
-    <row r="7" spans="1:14" s="10" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="32" t="s">
+    <row r="7" spans="1:30" s="10" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="32" t="s">
+      <c r="E7" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="F7" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="18" t="s">
+      <c r="G7" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="18" t="s">
+      <c r="H7" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="18" t="s">
+      <c r="I7" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="J7" s="37" t="s">
-        <v>32</v>
-      </c>
-      <c r="K7" s="39" t="s">
+      <c r="J7" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="K7" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="L7" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="M7" s="22"/>
-      <c r="N7" s="22"/>
+      <c r="L7" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="M7" s="24"/>
+      <c r="N7" s="24"/>
+      <c r="O7" s="24"/>
+      <c r="P7" s="24"/>
+      <c r="Q7" s="24"/>
+      <c r="R7" s="24"/>
+      <c r="S7" s="24"/>
+      <c r="T7" s="24"/>
+      <c r="U7" s="24"/>
+      <c r="V7" s="24"/>
+      <c r="W7" s="24"/>
+      <c r="X7" s="24"/>
+      <c r="Y7" s="24"/>
+      <c r="Z7" s="24"/>
+      <c r="AA7" s="24"/>
+      <c r="AB7" s="24"/>
+      <c r="AC7" s="24"/>
+      <c r="AD7" s="24"/>
     </row>
-    <row r="8" spans="1:14" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="33"/>
-      <c r="B8" s="33"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="38"/>
-      <c r="K8" s="40"/>
-      <c r="L8" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="M8" s="41" t="s">
+    <row r="8" spans="1:30" s="10" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="38"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="40"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="N8" s="23" t="s">
-        <v>34</v>
+      <c r="M8" s="29"/>
+      <c r="N8" s="29"/>
+      <c r="O8" s="29"/>
+      <c r="P8" s="29"/>
+      <c r="Q8" s="29"/>
+      <c r="R8" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="S8" s="29"/>
+      <c r="T8" s="29"/>
+      <c r="U8" s="29"/>
+      <c r="V8" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="W8" s="23"/>
+      <c r="X8" s="23"/>
+      <c r="Y8" s="23"/>
+      <c r="Z8" s="23"/>
+      <c r="AA8" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB8" s="26"/>
+      <c r="AC8" s="27"/>
+      <c r="AD8" s="23" t="s">
+        <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:14" s="10" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="34"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="38"/>
-      <c r="K9" s="40"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="41"/>
-      <c r="N9" s="23"/>
+    <row r="9" spans="1:30" s="10" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="A9" s="38"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="M9" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="N9" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="O9" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="P9" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q9" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="R9" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="S9" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="T9" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="U9" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="V9" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="W9" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="X9" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y9" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z9" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA9" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB9" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC9" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="AD9" s="23"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f>ROW()-9</f>
         <v>1</v>
@@ -1071,45 +1208,169 @@
       <c r="I10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J10" s="16" t="s">
+      <c r="J10" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="K10" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="L10" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="M10" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="N10" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="K10" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="L10" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="M10" s="17" t="s">
+      <c r="O10" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="P10" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q10" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="R10" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="S10" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="T10" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="U10" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="V10" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="W10" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="X10" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y10" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z10" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA10" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB10" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC10" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AD10" s="22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="N10" s="17" t="s">
-        <v>35</v>
+      <c r="K11" s="13">
+        <f ca="1">SUM( K10                               : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
+        <v>0</v>
+      </c>
+      <c r="L11" s="13">
+        <f ca="1">SUM( L10                               : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
+        <v>0</v>
+      </c>
+      <c r="M11" s="13">
+        <f ca="1">SUM( M10                               : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
+        <v>0</v>
+      </c>
+      <c r="N11" s="13">
+        <f ca="1">SUM( N10                               : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
+        <v>0</v>
+      </c>
+      <c r="O11" s="13">
+        <f ca="1">SUM( O10                               : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
+        <v>0</v>
+      </c>
+      <c r="P11" s="13">
+        <f ca="1">SUM( P10                               : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
+        <v>0</v>
+      </c>
+      <c r="Q11" s="13">
+        <f ca="1">SUM( Q10                               : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
+        <v>0</v>
+      </c>
+      <c r="R11" s="13">
+        <f ca="1">SUM( R10                               : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
+        <v>0</v>
+      </c>
+      <c r="S11" s="13">
+        <f ca="1">SUM( S10                               : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
+        <v>0</v>
+      </c>
+      <c r="T11" s="13">
+        <f ca="1">SUM( T10                               : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
+        <v>0</v>
+      </c>
+      <c r="U11" s="13">
+        <f ca="1">SUM( U10                               : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
+        <v>0</v>
+      </c>
+      <c r="V11" s="13">
+        <f ca="1">SUM( V10                               : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
+        <v>0</v>
+      </c>
+      <c r="W11" s="13">
+        <f ca="1">SUM( W10                               : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
+        <v>0</v>
+      </c>
+      <c r="X11" s="13">
+        <f ca="1">SUM( X10                               : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
+        <v>0</v>
+      </c>
+      <c r="Y11" s="13">
+        <f ca="1">SUM( Y10                               : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
+        <v>0</v>
+      </c>
+      <c r="Z11" s="13">
+        <f ca="1">SUM( Z10                               : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
+        <v>0</v>
+      </c>
+      <c r="AA11" s="13">
+        <f ca="1">SUM( AA10                               : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
+        <v>0</v>
+      </c>
+      <c r="AB11" s="13">
+        <f ca="1">SUM( AB10                               : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
+        <v>0</v>
+      </c>
+      <c r="AC11" s="13">
+        <f ca="1">SUM( AC10                               : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
+        <v>0</v>
+      </c>
+      <c r="AD11" s="13">
+        <f ca="1">SUM( AD10                               : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
+        <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="J11" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="K11" s="14">
-        <f ca="1">SUM( K10                             : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
-        <v>0</v>
-      </c>
-      <c r="L11" s="14">
-        <f ca="1">SUM( L10                             : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
-        <v>0</v>
-      </c>
-      <c r="M11" s="14">
-        <f ca="1">SUM( M10                             : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
-        <v>0</v>
-      </c>
-      <c r="N11" s="14">
-        <f ca="1">SUM( N10                             : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
-        <v>0</v>
-      </c>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="Z14" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="21">
     <mergeCell ref="A1:M1"/>
     <mergeCell ref="A2:M2"/>
     <mergeCell ref="A3:M3"/>
@@ -1121,14 +1382,16 @@
     <mergeCell ref="E7:E9"/>
     <mergeCell ref="J7:J9"/>
     <mergeCell ref="K7:K9"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="M8:M9"/>
     <mergeCell ref="F7:F9"/>
     <mergeCell ref="G7:G9"/>
     <mergeCell ref="H7:H9"/>
-    <mergeCell ref="L7:N7"/>
-    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="V8:Z8"/>
+    <mergeCell ref="AD8:AD9"/>
+    <mergeCell ref="L7:AD7"/>
+    <mergeCell ref="AA8:AC8"/>
     <mergeCell ref="I7:I9"/>
+    <mergeCell ref="L8:Q8"/>
+    <mergeCell ref="R8:U8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1137,7 +1400,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
@@ -1145,14 +1408,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:2" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>0</v>
       </c>

</xml_diff>